<commit_message>
added week 2 day 2
</commit_message>
<xml_diff>
--- a/TOC/ASDE 2023 - Day-wise ToC.xlsx
+++ b/TOC/ASDE 2023 - Day-wise ToC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online Training\ACE\Sapient\ASDE 2023\TOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF90A75F-FEEE-41AF-9FB6-F73F72DAA863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2784635-FB69-433F-8581-D6AE01BC19E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26702,8 +26702,8 @@
   <dimension ref="A1:M1803"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C160" sqref="C160"/>
+      <pane ySplit="2" topLeftCell="A507" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C524" sqref="C524"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
added week 2 day 3
</commit_message>
<xml_diff>
--- a/TOC/ASDE 2023 - Day-wise ToC.xlsx
+++ b/TOC/ASDE 2023 - Day-wise ToC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online Training\ACE\Sapient\ASDE 2023\TOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2784635-FB69-433F-8581-D6AE01BC19E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A3B242-5C47-48C2-A613-B13DE41145C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10236,6 +10236,18 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -10250,18 +10262,6 @@
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -25563,10 +25563,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="116" t="s">
         <v>988</v>
       </c>
-      <c r="B1" s="122"/>
+      <c r="B1" s="117"/>
       <c r="G1" s="5"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
@@ -25589,10 +25589,10 @@
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="15.6">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="118" t="s">
         <v>990</v>
       </c>
-      <c r="B3" s="124"/>
+      <c r="B3" s="119"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -25610,7 +25610,7 @@
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:12" ht="19.2" customHeight="1">
-      <c r="A6" s="118" t="s">
+      <c r="A6" s="122" t="s">
         <v>992</v>
       </c>
       <c r="B6" s="39" t="s">
@@ -25618,19 +25618,19 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A7" s="118"/>
+      <c r="A7" s="122"/>
       <c r="B7" s="43" t="s">
         <v>994</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A8" s="118"/>
+      <c r="A8" s="122"/>
       <c r="B8" s="39" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A9" s="118"/>
+      <c r="A9" s="122"/>
       <c r="B9" s="43" t="s">
         <v>2599</v>
       </c>
@@ -25652,7 +25652,7 @@
       <c r="B12" s="39"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="118" t="s">
+      <c r="A13" s="122" t="s">
         <v>992</v>
       </c>
       <c r="B13" s="39" t="s">
@@ -25660,51 +25660,51 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="118"/>
+      <c r="A14" s="122"/>
       <c r="B14" s="43" t="s">
         <v>1712</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="118"/>
+      <c r="A15" s="122"/>
       <c r="B15" s="12" t="s">
         <v>1002</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="118"/>
+      <c r="A16" s="122"/>
       <c r="B16" s="12" t="s">
         <v>1003</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="118"/>
+      <c r="A17" s="122"/>
       <c r="B17" s="39" t="s">
         <v>2594</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="118"/>
+      <c r="A18" s="122"/>
       <c r="B18" s="12" t="s">
         <v>1006</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="118"/>
+      <c r="A19" s="122"/>
       <c r="B19" s="39" t="s">
         <v>1711</v>
       </c>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="118"/>
+      <c r="A20" s="122"/>
       <c r="B20" s="35" t="s">
         <v>2130</v>
       </c>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="118"/>
+      <c r="A21" s="122"/>
       <c r="B21" s="11" t="s">
         <v>998</v>
       </c>
@@ -25726,7 +25726,7 @@
       <c r="B24" s="39"/>
     </row>
     <row r="25" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A25" s="118" t="s">
+      <c r="A25" s="122" t="s">
         <v>992</v>
       </c>
       <c r="B25" s="39" t="s">
@@ -25734,7 +25734,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A26" s="118"/>
+      <c r="A26" s="122"/>
       <c r="B26" s="43" t="s">
         <v>2129</v>
       </c>
@@ -25770,10 +25770,10 @@
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" ht="15.6">
-      <c r="A32" s="123" t="s">
+      <c r="A32" s="118" t="s">
         <v>1007</v>
       </c>
-      <c r="B32" s="124"/>
+      <c r="B32" s="119"/>
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" ht="15.6">
@@ -25818,7 +25818,7 @@
       <c r="A39" s="3"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A40" s="118" t="s">
+      <c r="A40" s="122" t="s">
         <v>992</v>
       </c>
       <c r="B40" s="42" t="s">
@@ -25826,43 +25826,43 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A41" s="118"/>
+      <c r="A41" s="122"/>
       <c r="B41" s="12" t="s">
         <v>1015</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A42" s="118"/>
+      <c r="A42" s="122"/>
       <c r="B42" s="42" t="s">
         <v>1016</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A43" s="118"/>
+      <c r="A43" s="122"/>
       <c r="B43" s="12" t="s">
         <v>1017</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A44" s="118"/>
+      <c r="A44" s="122"/>
       <c r="B44" s="42" t="s">
         <v>1018</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A45" s="118"/>
+      <c r="A45" s="122"/>
       <c r="B45" s="12" t="s">
         <v>1019</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A46" s="118"/>
+      <c r="A46" s="122"/>
       <c r="B46" s="42" t="s">
         <v>1730</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.6" customHeight="1">
-      <c r="A47" s="118"/>
+      <c r="A47" s="122"/>
       <c r="B47" s="12" t="s">
         <v>1729</v>
       </c>
@@ -25890,7 +25890,7 @@
       <c r="B51" s="42"/>
     </row>
     <row r="52" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A52" s="118" t="s">
+      <c r="A52" s="122" t="s">
         <v>992</v>
       </c>
       <c r="B52" s="42" t="s">
@@ -25898,25 +25898,25 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A53" s="118"/>
+      <c r="A53" s="122"/>
       <c r="B53" s="12" t="s">
         <v>1009</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A54" s="118"/>
+      <c r="A54" s="122"/>
       <c r="B54" s="42" t="s">
         <v>1011</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A55" s="118"/>
+      <c r="A55" s="122"/>
       <c r="B55" s="11" t="s">
         <v>1012</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="118"/>
+      <c r="A56" s="122"/>
     </row>
     <row r="57" spans="1:2" ht="15.75" customHeight="1">
       <c r="B57" s="42" t="s">
@@ -25955,10 +25955,10 @@
       <c r="B64" s="9"/>
     </row>
     <row r="65" spans="1:2" ht="15.6">
-      <c r="A65" s="116" t="s">
+      <c r="A65" s="120" t="s">
         <v>1025</v>
       </c>
-      <c r="B65" s="117"/>
+      <c r="B65" s="121"/>
     </row>
     <row r="66" spans="1:2" ht="15.6">
       <c r="A66" s="97"/>
@@ -25981,7 +25981,7 @@
       <c r="B69" s="13"/>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="118" t="s">
+      <c r="A70" s="122" t="s">
         <v>992</v>
       </c>
       <c r="B70" s="101" t="s">
@@ -25989,7 +25989,7 @@
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="118"/>
+      <c r="A71" s="122"/>
       <c r="B71" s="11" t="s">
         <v>1028</v>
       </c>
@@ -26015,7 +26015,7 @@
       <c r="B75" s="101"/>
     </row>
     <row r="76" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A76" s="118" t="s">
+      <c r="A76" s="122" t="s">
         <v>992</v>
       </c>
       <c r="B76" s="11" t="s">
@@ -26023,7 +26023,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A77" s="118"/>
+      <c r="A77" s="122"/>
       <c r="B77" s="11" t="s">
         <v>1034</v>
       </c>
@@ -26046,7 +26046,7 @@
       <c r="B81" s="42"/>
     </row>
     <row r="82" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A82" s="118" t="s">
+      <c r="A82" s="122" t="s">
         <v>992</v>
       </c>
       <c r="B82" s="42" t="s">
@@ -26054,19 +26054,19 @@
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A83" s="118"/>
+      <c r="A83" s="122"/>
       <c r="B83" s="11" t="s">
         <v>1037</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A84" s="118"/>
+      <c r="A84" s="122"/>
       <c r="B84" s="42" t="s">
         <v>1038</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A85" s="118"/>
+      <c r="A85" s="122"/>
       <c r="B85" s="11" t="s">
         <v>1039</v>
       </c>
@@ -26102,7 +26102,7 @@
       <c r="B91" s="42"/>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" s="118" t="s">
+      <c r="A92" s="122" t="s">
         <v>992</v>
       </c>
       <c r="B92" s="42" t="s">
@@ -26110,7 +26110,7 @@
       </c>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" s="118"/>
+      <c r="A93" s="122"/>
       <c r="B93" s="35" t="s">
         <v>1039</v>
       </c>
@@ -26142,10 +26142,10 @@
       <c r="B98" s="14"/>
     </row>
     <row r="99" spans="1:2" ht="15.6">
-      <c r="A99" s="116" t="s">
+      <c r="A99" s="120" t="s">
         <v>1061</v>
       </c>
-      <c r="B99" s="117"/>
+      <c r="B99" s="121"/>
     </row>
     <row r="100" spans="1:2" ht="15.6">
       <c r="A100" s="97"/>
@@ -26164,7 +26164,7 @@
       <c r="B102" s="42"/>
     </row>
     <row r="103" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A103" s="118" t="s">
+      <c r="A103" s="122" t="s">
         <v>992</v>
       </c>
       <c r="B103" s="42" t="s">
@@ -26172,59 +26172,59 @@
       </c>
     </row>
     <row r="104" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A104" s="118"/>
+      <c r="A104" s="122"/>
       <c r="B104" s="11" t="s">
         <v>1075</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A105" s="118"/>
+      <c r="A105" s="122"/>
       <c r="B105" s="11" t="s">
         <v>1076</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A106" s="118"/>
+      <c r="A106" s="122"/>
       <c r="B106" s="11" t="s">
         <v>1077</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="1.95" customHeight="1">
-      <c r="A107" s="118"/>
+      <c r="A107" s="122"/>
       <c r="B107" s="11"/>
     </row>
     <row r="108" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A108" s="118"/>
+      <c r="A108" s="122"/>
       <c r="B108" s="11" t="s">
         <v>1078</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A109" s="118"/>
+      <c r="A109" s="122"/>
       <c r="B109" s="42" t="s">
         <v>1069</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="19.8" customHeight="1">
-      <c r="A110" s="118"/>
+      <c r="A110" s="122"/>
       <c r="B110" s="11" t="s">
         <v>1079</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A111" s="118"/>
+      <c r="A111" s="122"/>
       <c r="B111" s="42" t="s">
         <v>785</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A112" s="118"/>
+      <c r="A112" s="122"/>
       <c r="B112" s="11" t="s">
         <v>1080</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A113" s="118"/>
+      <c r="A113" s="122"/>
       <c r="B113" s="11" t="s">
         <v>1081</v>
       </c>
@@ -26245,7 +26245,7 @@
       <c r="B116" s="18"/>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="118" t="s">
+      <c r="A117" s="122" t="s">
         <v>992</v>
       </c>
       <c r="B117" s="42" t="s">
@@ -26253,25 +26253,25 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A118" s="118"/>
+      <c r="A118" s="122"/>
       <c r="B118" s="11" t="s">
         <v>1088</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A119" s="118"/>
+      <c r="A119" s="122"/>
       <c r="B119" s="11" t="s">
         <v>1089</v>
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="118"/>
+      <c r="A120" s="122"/>
       <c r="B120" s="11" t="s">
         <v>1090</v>
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="118"/>
+      <c r="A121" s="122"/>
       <c r="B121" s="11" t="s">
         <v>1091</v>
       </c>
@@ -26291,7 +26291,7 @@
       <c r="B124" s="18"/>
     </row>
     <row r="125" spans="1:3" ht="18">
-      <c r="A125" s="118" t="s">
+      <c r="A125" s="122" t="s">
         <v>992</v>
       </c>
       <c r="B125" s="18" t="s">
@@ -26299,7 +26299,7 @@
       </c>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="118"/>
+      <c r="A126" s="122"/>
       <c r="B126" s="35" t="s">
         <v>2223</v>
       </c>
@@ -26334,10 +26334,10 @@
       <c r="B131" s="3"/>
     </row>
     <row r="132" spans="1:3" ht="15.6">
-      <c r="A132" s="119" t="s">
+      <c r="A132" s="123" t="s">
         <v>1093</v>
       </c>
-      <c r="B132" s="117"/>
+      <c r="B132" s="121"/>
     </row>
     <row r="133" spans="1:3" ht="15.6">
       <c r="A133" s="97"/>
@@ -26356,7 +26356,7 @@
       <c r="B135" s="104"/>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" s="118" t="s">
+      <c r="A136" s="122" t="s">
         <v>992</v>
       </c>
       <c r="B136" s="42" t="s">
@@ -26364,31 +26364,31 @@
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A137" s="118"/>
+      <c r="A137" s="122"/>
       <c r="B137" s="35" t="s">
         <v>2539</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A138" s="118"/>
+      <c r="A138" s="122"/>
       <c r="B138" s="11" t="s">
         <v>1094</v>
       </c>
     </row>
     <row r="139" spans="1:3">
-      <c r="A139" s="118"/>
+      <c r="A139" s="122"/>
       <c r="B139" s="35" t="s">
         <v>2579</v>
       </c>
     </row>
     <row r="140" spans="1:3">
-      <c r="A140" s="118"/>
+      <c r="A140" s="122"/>
       <c r="B140" s="35" t="s">
         <v>2580</v>
       </c>
     </row>
     <row r="141" spans="1:3">
-      <c r="A141" s="118"/>
+      <c r="A141" s="122"/>
       <c r="B141" s="35" t="s">
         <v>2595</v>
       </c>
@@ -26432,7 +26432,7 @@
       <c r="B148" s="9"/>
     </row>
     <row r="149" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A149" s="120" t="s">
+      <c r="A149" s="124" t="s">
         <v>992</v>
       </c>
       <c r="B149" s="16" t="s">
@@ -26440,177 +26440,177 @@
       </c>
     </row>
     <row r="150" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A150" s="118"/>
+      <c r="A150" s="122"/>
       <c r="B150" s="11" t="s">
         <v>1102</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A151" s="118"/>
+      <c r="A151" s="122"/>
       <c r="B151" s="11" t="s">
         <v>1103</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A152" s="118"/>
+      <c r="A152" s="122"/>
       <c r="B152" s="11" t="s">
         <v>1104</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A153" s="118"/>
+      <c r="A153" s="122"/>
       <c r="B153" s="11" t="s">
         <v>1105</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A154" s="118"/>
+      <c r="A154" s="122"/>
       <c r="B154" s="11" t="s">
         <v>1106</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A155" s="118"/>
+      <c r="A155" s="122"/>
       <c r="B155" s="11" t="s">
         <v>1107</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A156" s="118"/>
+      <c r="A156" s="122"/>
       <c r="B156" s="11" t="s">
         <v>1108</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A157" s="118"/>
+      <c r="A157" s="122"/>
       <c r="B157" s="11" t="s">
         <v>1109</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A158" s="118"/>
+      <c r="A158" s="122"/>
       <c r="B158" s="11" t="s">
         <v>1110</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A159" s="118"/>
+      <c r="A159" s="122"/>
       <c r="B159" s="11" t="s">
         <v>1111</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A160" s="118"/>
+      <c r="A160" s="122"/>
       <c r="B160" s="11" t="s">
         <v>1112</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A161" s="118"/>
+      <c r="A161" s="122"/>
       <c r="B161" s="11" t="s">
         <v>1113</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A162" s="118"/>
+      <c r="A162" s="122"/>
       <c r="B162" s="11" t="s">
         <v>1114</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A163" s="118"/>
+      <c r="A163" s="122"/>
       <c r="B163" s="11" t="s">
         <v>1115</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A164" s="118"/>
+      <c r="A164" s="122"/>
       <c r="B164" s="11" t="s">
         <v>1116</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A165" s="118"/>
+      <c r="A165" s="122"/>
       <c r="B165" s="11" t="s">
         <v>1117</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A166" s="118"/>
+      <c r="A166" s="122"/>
       <c r="B166" s="11" t="s">
         <v>1118</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A167" s="118"/>
+      <c r="A167" s="122"/>
       <c r="B167" s="11" t="s">
         <v>1119</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A168" s="118"/>
+      <c r="A168" s="122"/>
       <c r="B168" s="11" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A169" s="118"/>
+      <c r="A169" s="122"/>
       <c r="B169" s="11" t="s">
         <v>1121</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A170" s="118"/>
+      <c r="A170" s="122"/>
       <c r="B170" s="11" t="s">
         <v>1122</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A171" s="118"/>
+      <c r="A171" s="122"/>
       <c r="B171" s="11" t="s">
         <v>1123</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A172" s="118"/>
+      <c r="A172" s="122"/>
       <c r="B172" s="11"/>
     </row>
     <row r="173" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A173" s="118"/>
+      <c r="A173" s="122"/>
       <c r="B173" s="35" t="s">
         <v>2584</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A174" s="118"/>
+      <c r="A174" s="122"/>
       <c r="B174" s="35"/>
     </row>
     <row r="175" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A175" s="118"/>
+      <c r="A175" s="122"/>
       <c r="B175" s="35" t="s">
         <v>2585</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A176" s="118"/>
+      <c r="A176" s="122"/>
       <c r="B176" s="35" t="s">
         <v>2587</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A177" s="118"/>
+      <c r="A177" s="122"/>
       <c r="B177" s="35" t="s">
         <v>2590</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A178" s="118"/>
+      <c r="A178" s="122"/>
       <c r="B178" s="35" t="s">
         <v>2597</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A179" s="118"/>
+      <c r="A179" s="122"/>
       <c r="B179" s="35" t="s">
         <v>2598</v>
       </c>
@@ -26665,11 +26665,21 @@
       </c>
     </row>
     <row r="189" spans="1:2" ht="15.6">
-      <c r="A189" s="116"/>
-      <c r="B189" s="117"/>
+      <c r="A189" s="120"/>
+      <c r="B189" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A189:B189"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="A117:A121"/>
+    <mergeCell ref="A103:A113"/>
+    <mergeCell ref="A136:A141"/>
+    <mergeCell ref="A149:A179"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A32:B32"/>
@@ -26681,16 +26691,6 @@
     <mergeCell ref="A76:A77"/>
     <mergeCell ref="A52:A56"/>
     <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A189:B189"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="A117:A121"/>
-    <mergeCell ref="A103:A113"/>
-    <mergeCell ref="A136:A141"/>
-    <mergeCell ref="A149:A179"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -26702,8 +26702,8 @@
   <dimension ref="A1:M1803"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A507" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C524" sqref="C524"/>
+      <pane ySplit="2" topLeftCell="A575" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C567" sqref="C567"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -26716,11 +26716,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="116" t="s">
         <v>988</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
       <c r="H1" s="5"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
@@ -26746,11 +26746,11 @@
       <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" ht="12" customHeight="1">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="118" t="s">
         <v>990</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -27224,7 +27224,7 @@
       <c r="C82" s="12"/>
     </row>
     <row r="83" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B83" s="118" t="s">
+      <c r="B83" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C83" s="39" t="s">
@@ -27232,143 +27232,143 @@
       </c>
     </row>
     <row r="84" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B84" s="118"/>
+      <c r="B84" s="122"/>
       <c r="C84" s="12" t="s">
         <v>994</v>
       </c>
     </row>
     <row r="85" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B85" s="118"/>
+      <c r="B85" s="122"/>
       <c r="C85" s="39" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="86" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B86" s="118"/>
+      <c r="B86" s="122"/>
       <c r="C86" s="43" t="s">
         <v>2672</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B87" s="118"/>
+      <c r="B87" s="122"/>
       <c r="C87" s="39" t="s">
         <v>2653</v>
       </c>
     </row>
     <row r="88" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B88" s="118"/>
+      <c r="B88" s="122"/>
       <c r="C88" s="12" t="s">
         <v>2663</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B89" s="118"/>
+      <c r="B89" s="122"/>
       <c r="C89" s="43" t="s">
         <v>2664</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B90" s="118"/>
+      <c r="B90" s="122"/>
       <c r="C90" s="12" t="s">
         <v>2665</v>
       </c>
     </row>
     <row r="91" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B91" s="118"/>
+      <c r="B91" s="122"/>
       <c r="C91" s="114" t="s">
         <v>2654</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B92" s="118"/>
+      <c r="B92" s="122"/>
       <c r="C92" s="114" t="s">
         <v>2655</v>
       </c>
     </row>
     <row r="93" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B93" s="118"/>
+      <c r="B93" s="122"/>
       <c r="C93" s="114" t="s">
         <v>2656</v>
       </c>
     </row>
     <row r="94" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B94" s="118"/>
+      <c r="B94" s="122"/>
       <c r="C94" s="39" t="s">
         <v>2658</v>
       </c>
     </row>
     <row r="95" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B95" s="118"/>
+      <c r="B95" s="122"/>
       <c r="C95" s="114" t="s">
         <v>2657</v>
       </c>
     </row>
     <row r="96" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B96" s="118"/>
+      <c r="B96" s="122"/>
       <c r="C96" t="s">
         <v>2659</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B97" s="118"/>
+      <c r="B97" s="122"/>
       <c r="C97" s="39" t="s">
         <v>2673</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B98" s="118"/>
+      <c r="B98" s="122"/>
       <c r="C98" s="43" t="s">
         <v>2660</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B99" s="118"/>
+      <c r="B99" s="122"/>
       <c r="C99" s="43" t="s">
         <v>2661</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B100" s="118"/>
+      <c r="B100" s="122"/>
       <c r="C100" s="43" t="s">
         <v>2662</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B101" s="118"/>
+      <c r="B101" s="122"/>
       <c r="C101" s="39" t="s">
         <v>2668</v>
       </c>
     </row>
     <row r="102" spans="1:9">
-      <c r="B102" s="118"/>
+      <c r="B102" s="122"/>
       <c r="C102" s="43" t="s">
         <v>2666</v>
       </c>
       <c r="I102" s="2"/>
     </row>
     <row r="103" spans="1:9">
-      <c r="B103" s="118"/>
+      <c r="B103" s="122"/>
       <c r="C103" s="43" t="s">
         <v>2667</v>
       </c>
       <c r="I103" s="2"/>
     </row>
     <row r="104" spans="1:9">
-      <c r="B104" s="118"/>
+      <c r="B104" s="122"/>
       <c r="C104" s="39" t="s">
         <v>2670</v>
       </c>
       <c r="I104" s="2"/>
     </row>
     <row r="105" spans="1:9">
-      <c r="B105" s="118"/>
+      <c r="B105" s="122"/>
       <c r="C105" s="115" t="s">
         <v>2669</v>
       </c>
       <c r="I105" s="2"/>
     </row>
     <row r="106" spans="1:9">
-      <c r="B106" s="118"/>
+      <c r="B106" s="122"/>
       <c r="C106" s="115" t="s">
         <v>2671</v>
       </c>
@@ -27735,7 +27735,7 @@
       <c r="I168" s="2"/>
     </row>
     <row r="169" spans="2:9">
-      <c r="B169" s="118" t="s">
+      <c r="B169" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C169" s="39" t="s">
@@ -27744,21 +27744,21 @@
       <c r="I169" s="2"/>
     </row>
     <row r="170" spans="2:9">
-      <c r="B170" s="118"/>
+      <c r="B170" s="122"/>
       <c r="C170" s="43" t="s">
         <v>1712</v>
       </c>
       <c r="I170" s="2"/>
     </row>
     <row r="171" spans="2:9">
-      <c r="B171" s="118"/>
+      <c r="B171" s="122"/>
       <c r="C171" s="12" t="s">
         <v>1002</v>
       </c>
       <c r="I171" s="2"/>
     </row>
     <row r="172" spans="2:9">
-      <c r="B172" s="118"/>
+      <c r="B172" s="122"/>
       <c r="C172" s="12" t="s">
         <v>1003</v>
       </c>
@@ -27878,7 +27878,7 @@
       <c r="I192" s="2"/>
     </row>
     <row r="193" spans="1:9" ht="14.4" customHeight="1">
-      <c r="B193" s="118" t="s">
+      <c r="B193" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C193" s="39" t="s">
@@ -27887,28 +27887,28 @@
       <c r="I193" s="2"/>
     </row>
     <row r="194" spans="1:9" ht="14.4" customHeight="1">
-      <c r="B194" s="118"/>
+      <c r="B194" s="122"/>
       <c r="C194" s="12" t="s">
         <v>1006</v>
       </c>
       <c r="I194" s="2"/>
     </row>
     <row r="195" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B195" s="118"/>
+      <c r="B195" s="122"/>
       <c r="C195" s="39" t="s">
         <v>1711</v>
       </c>
       <c r="I195" s="2"/>
     </row>
     <row r="196" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B196" s="118"/>
+      <c r="B196" s="122"/>
       <c r="C196" s="35" t="s">
         <v>2130</v>
       </c>
       <c r="I196" s="2"/>
     </row>
     <row r="197" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B197" s="118"/>
+      <c r="B197" s="122"/>
       <c r="C197" s="11" t="s">
         <v>998</v>
       </c>
@@ -28262,7 +28262,7 @@
       <c r="I245" s="2"/>
     </row>
     <row r="246" spans="1:9">
-      <c r="B246" s="118" t="s">
+      <c r="B246" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C246" s="39" t="s">
@@ -28271,7 +28271,7 @@
       <c r="I246" s="2"/>
     </row>
     <row r="247" spans="1:9">
-      <c r="B247" s="118"/>
+      <c r="B247" s="122"/>
       <c r="C247" s="43" t="s">
         <v>2129</v>
       </c>
@@ -28783,11 +28783,11 @@
       <c r="I350" s="2"/>
     </row>
     <row r="351" spans="1:9" ht="15.6">
-      <c r="A351" s="123" t="s">
+      <c r="A351" s="118" t="s">
         <v>1007</v>
       </c>
-      <c r="B351" s="123"/>
-      <c r="C351" s="123"/>
+      <c r="B351" s="118"/>
+      <c r="C351" s="118"/>
       <c r="I351" s="2"/>
     </row>
     <row r="352" spans="1:9" ht="15">
@@ -29815,7 +29815,7 @@
       <c r="C543" s="12"/>
     </row>
     <row r="544" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B544" s="118" t="s">
+      <c r="B544" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C544" s="42" t="s">
@@ -29823,43 +29823,43 @@
       </c>
     </row>
     <row r="545" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B545" s="118"/>
+      <c r="B545" s="122"/>
       <c r="C545" s="12" t="s">
         <v>1015</v>
       </c>
     </row>
     <row r="546" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B546" s="118"/>
+      <c r="B546" s="122"/>
       <c r="C546" s="42" t="s">
         <v>1016</v>
       </c>
     </row>
     <row r="547" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B547" s="118"/>
+      <c r="B547" s="122"/>
       <c r="C547" s="12" t="s">
         <v>1017</v>
       </c>
     </row>
     <row r="548" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B548" s="118"/>
+      <c r="B548" s="122"/>
       <c r="C548" s="42" t="s">
         <v>1018</v>
       </c>
     </row>
     <row r="549" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B549" s="118"/>
+      <c r="B549" s="122"/>
       <c r="C549" s="12" t="s">
         <v>1019</v>
       </c>
     </row>
     <row r="550" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B550" s="118"/>
+      <c r="B550" s="122"/>
       <c r="C550" s="42" t="s">
         <v>1730</v>
       </c>
     </row>
     <row r="551" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B551" s="118"/>
+      <c r="B551" s="122"/>
       <c r="C551" s="12" t="s">
         <v>1729</v>
       </c>
@@ -29914,7 +29914,7 @@
       <c r="C560" s="12"/>
     </row>
     <row r="561" spans="1:9" ht="14.4" customHeight="1">
-      <c r="B561" s="118" t="s">
+      <c r="B561" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C561" s="42" t="s">
@@ -29922,25 +29922,25 @@
       </c>
     </row>
     <row r="562" spans="1:9" ht="14.4" customHeight="1">
-      <c r="B562" s="118"/>
+      <c r="B562" s="122"/>
       <c r="C562" s="12" t="s">
         <v>1009</v>
       </c>
     </row>
     <row r="563" spans="1:9">
-      <c r="B563" s="118"/>
+      <c r="B563" s="122"/>
       <c r="C563" s="42" t="s">
         <v>1011</v>
       </c>
     </row>
     <row r="564" spans="1:9" ht="14.4" customHeight="1">
-      <c r="B564" s="118"/>
+      <c r="B564" s="122"/>
       <c r="C564" s="11" t="s">
         <v>1012</v>
       </c>
     </row>
     <row r="565" spans="1:9" ht="14.4" customHeight="1">
-      <c r="B565" s="118"/>
+      <c r="B565" s="122"/>
     </row>
     <row r="566" spans="1:9" ht="15.6">
       <c r="B566" s="10"/>
@@ -30690,11 +30690,11 @@
       <c r="C698" s="11"/>
     </row>
     <row r="699" spans="1:3" ht="13.8" customHeight="1">
-      <c r="A699" s="123" t="s">
+      <c r="A699" s="118" t="s">
         <v>1025</v>
       </c>
-      <c r="B699" s="123"/>
-      <c r="C699" s="123"/>
+      <c r="B699" s="118"/>
+      <c r="C699" s="118"/>
     </row>
     <row r="700" spans="1:3" ht="15.6">
       <c r="A700" s="99"/>
@@ -30943,7 +30943,7 @@
       <c r="C747" s="11"/>
     </row>
     <row r="748" spans="1:3">
-      <c r="B748" s="118" t="s">
+      <c r="B748" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C748" s="42" t="s">
@@ -30951,7 +30951,7 @@
       </c>
     </row>
     <row r="749" spans="1:3">
-      <c r="B749" s="118"/>
+      <c r="B749" s="122"/>
       <c r="C749" s="11" t="s">
         <v>1028</v>
       </c>
@@ -31060,7 +31060,7 @@
       <c r="D769" s="112"/>
     </row>
     <row r="770" spans="1:4">
-      <c r="B770" s="118" t="s">
+      <c r="B770" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C770" s="101" t="s">
@@ -31068,13 +31068,13 @@
       </c>
     </row>
     <row r="771" spans="1:4">
-      <c r="B771" s="118"/>
+      <c r="B771" s="122"/>
       <c r="C771" s="35" t="s">
         <v>1033</v>
       </c>
     </row>
     <row r="772" spans="1:4">
-      <c r="B772" s="118"/>
+      <c r="B772" s="122"/>
       <c r="C772" s="35" t="s">
         <v>1034</v>
       </c>
@@ -31253,7 +31253,7 @@
       <c r="C806" s="35"/>
     </row>
     <row r="807" spans="1:4">
-      <c r="B807" s="118" t="s">
+      <c r="B807" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C807" s="42" t="s">
@@ -31261,7 +31261,7 @@
       </c>
     </row>
     <row r="808" spans="1:4">
-      <c r="B808" s="118"/>
+      <c r="B808" s="122"/>
       <c r="C808" s="35" t="s">
         <v>1037</v>
       </c>
@@ -31811,7 +31811,7 @@
       <c r="C919" s="42"/>
     </row>
     <row r="920" spans="1:3">
-      <c r="B920" s="118" t="s">
+      <c r="B920" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C920" s="42" t="s">
@@ -31819,7 +31819,7 @@
       </c>
     </row>
     <row r="921" spans="1:3">
-      <c r="B921" s="118"/>
+      <c r="B921" s="122"/>
       <c r="C921" s="35" t="s">
         <v>1039</v>
       </c>
@@ -32685,11 +32685,11 @@
       <c r="C1097" s="35"/>
     </row>
     <row r="1098" spans="1:3" ht="15.6">
-      <c r="A1098" s="123" t="s">
+      <c r="A1098" s="118" t="s">
         <v>1061</v>
       </c>
-      <c r="B1098" s="123"/>
-      <c r="C1098" s="123"/>
+      <c r="B1098" s="118"/>
+      <c r="C1098" s="118"/>
     </row>
     <row r="1099" spans="1:3">
       <c r="C1099" s="35"/>
@@ -32788,7 +32788,7 @@
       <c r="C1118" s="35"/>
     </row>
     <row r="1119" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1119" s="118" t="s">
+      <c r="B1119" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C1119" s="42" t="s">
@@ -32796,56 +32796,56 @@
       </c>
     </row>
     <row r="1120" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1120" s="118"/>
+      <c r="B1120" s="122"/>
       <c r="C1120" s="35" t="s">
         <v>1075</v>
       </c>
     </row>
     <row r="1121" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1121" s="118"/>
+      <c r="B1121" s="122"/>
       <c r="C1121" s="35" t="s">
         <v>1076</v>
       </c>
     </row>
     <row r="1122" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1122" s="118"/>
+      <c r="B1122" s="122"/>
       <c r="C1122" s="35" t="s">
         <v>1077</v>
       </c>
     </row>
     <row r="1123" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1123" s="118"/>
+      <c r="B1123" s="122"/>
       <c r="C1123" s="35" t="s">
         <v>1078</v>
       </c>
     </row>
     <row r="1124" spans="1:4" ht="15.6" customHeight="1">
-      <c r="B1124" s="118"/>
+      <c r="B1124" s="122"/>
       <c r="C1124" s="42" t="s">
         <v>1069</v>
       </c>
     </row>
     <row r="1125" spans="1:4" ht="16.8" customHeight="1">
-      <c r="B1125" s="118"/>
+      <c r="B1125" s="122"/>
       <c r="C1125" s="35" t="s">
         <v>1079</v>
       </c>
     </row>
     <row r="1126" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1126" s="118"/>
+      <c r="B1126" s="122"/>
       <c r="C1126" s="42" t="s">
         <v>785</v>
       </c>
     </row>
     <row r="1127" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1127" s="118"/>
+      <c r="B1127" s="122"/>
       <c r="C1127" s="35" t="s">
         <v>1080</v>
       </c>
       <c r="D1127" s="108"/>
     </row>
     <row r="1128" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1128" s="118"/>
+      <c r="B1128" s="122"/>
       <c r="C1128" s="35" t="s">
         <v>1081</v>
       </c>
@@ -33213,7 +33213,7 @@
       <c r="C1201" s="35"/>
     </row>
     <row r="1202" spans="1:3" ht="18">
-      <c r="B1202" s="118" t="s">
+      <c r="B1202" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C1202" s="18" t="s">
@@ -33221,25 +33221,25 @@
       </c>
     </row>
     <row r="1203" spans="1:3">
-      <c r="B1203" s="118"/>
+      <c r="B1203" s="122"/>
       <c r="C1203" s="35" t="s">
         <v>1088</v>
       </c>
     </row>
     <row r="1204" spans="1:3">
-      <c r="B1204" s="118"/>
+      <c r="B1204" s="122"/>
       <c r="C1204" s="35" t="s">
         <v>1089</v>
       </c>
     </row>
     <row r="1205" spans="1:3">
-      <c r="B1205" s="118"/>
+      <c r="B1205" s="122"/>
       <c r="C1205" s="35" t="s">
         <v>1090</v>
       </c>
     </row>
     <row r="1206" spans="1:3">
-      <c r="B1206" s="118"/>
+      <c r="B1206" s="122"/>
       <c r="C1206" s="35" t="s">
         <v>1091</v>
       </c>
@@ -33776,7 +33776,7 @@
       <c r="C1300" s="42"/>
     </row>
     <row r="1301" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1301" s="118" t="s">
+      <c r="B1301" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C1301" s="42" t="s">
@@ -33784,7 +33784,7 @@
       </c>
     </row>
     <row r="1302" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1302" s="118"/>
+      <c r="B1302" s="122"/>
       <c r="C1302" s="35" t="s">
         <v>2538</v>
       </c>
@@ -34659,11 +34659,11 @@
       <c r="C1490" s="35"/>
     </row>
     <row r="1491" spans="1:4" ht="15.6">
-      <c r="A1491" s="123" t="s">
+      <c r="A1491" s="118" t="s">
         <v>1093</v>
       </c>
-      <c r="B1491" s="123"/>
-      <c r="C1491" s="123"/>
+      <c r="B1491" s="118"/>
+      <c r="C1491" s="118"/>
     </row>
     <row r="1492" spans="1:4" ht="15.6">
       <c r="A1492" s="99"/>
@@ -34996,7 +34996,7 @@
       <c r="C1548" s="35"/>
     </row>
     <row r="1549" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1549" s="118" t="s">
+      <c r="B1549" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C1549" s="42" t="s">
@@ -35004,31 +35004,31 @@
       </c>
     </row>
     <row r="1550" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1550" s="118"/>
+      <c r="B1550" s="122"/>
       <c r="C1550" s="35" t="s">
         <v>2539</v>
       </c>
     </row>
     <row r="1551" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1551" s="118"/>
+      <c r="B1551" s="122"/>
       <c r="C1551" s="11" t="s">
         <v>1094</v>
       </c>
     </row>
     <row r="1552" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B1552" s="118"/>
+      <c r="B1552" s="122"/>
       <c r="C1552" s="35" t="s">
         <v>2579</v>
       </c>
     </row>
     <row r="1553" spans="1:3" ht="15.6" customHeight="1">
-      <c r="B1553" s="118"/>
+      <c r="B1553" s="122"/>
       <c r="C1553" s="35" t="s">
         <v>2580</v>
       </c>
     </row>
     <row r="1554" spans="1:3" ht="15.6" customHeight="1">
-      <c r="B1554" s="118"/>
+      <c r="B1554" s="122"/>
       <c r="C1554" s="35" t="s">
         <v>2595</v>
       </c>
@@ -35782,7 +35782,7 @@
       <c r="C1697" s="11"/>
     </row>
     <row r="1698" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1698" s="118" t="s">
+      <c r="B1698" s="122" t="s">
         <v>992</v>
       </c>
       <c r="C1698" s="46" t="s">
@@ -35790,177 +35790,177 @@
       </c>
     </row>
     <row r="1699" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1699" s="118"/>
+      <c r="B1699" s="122"/>
       <c r="C1699" s="11" t="s">
         <v>1102</v>
       </c>
     </row>
     <row r="1700" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1700" s="118"/>
+      <c r="B1700" s="122"/>
       <c r="C1700" s="11" t="s">
         <v>1103</v>
       </c>
     </row>
     <row r="1701" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1701" s="118"/>
+      <c r="B1701" s="122"/>
       <c r="C1701" s="11" t="s">
         <v>1104</v>
       </c>
     </row>
     <row r="1702" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1702" s="118"/>
+      <c r="B1702" s="122"/>
       <c r="C1702" s="11" t="s">
         <v>1105</v>
       </c>
     </row>
     <row r="1703" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1703" s="118"/>
+      <c r="B1703" s="122"/>
       <c r="C1703" s="11" t="s">
         <v>1106</v>
       </c>
     </row>
     <row r="1704" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1704" s="118"/>
+      <c r="B1704" s="122"/>
       <c r="C1704" s="11" t="s">
         <v>1107</v>
       </c>
     </row>
     <row r="1705" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1705" s="118"/>
+      <c r="B1705" s="122"/>
       <c r="C1705" s="11" t="s">
         <v>1108</v>
       </c>
     </row>
     <row r="1706" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1706" s="118"/>
+      <c r="B1706" s="122"/>
       <c r="C1706" s="11" t="s">
         <v>1109</v>
       </c>
     </row>
     <row r="1707" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1707" s="118"/>
+      <c r="B1707" s="122"/>
       <c r="C1707" s="11" t="s">
         <v>1110</v>
       </c>
     </row>
     <row r="1708" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1708" s="118"/>
+      <c r="B1708" s="122"/>
       <c r="C1708" s="11" t="s">
         <v>1111</v>
       </c>
     </row>
     <row r="1709" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1709" s="118"/>
+      <c r="B1709" s="122"/>
       <c r="C1709" s="11" t="s">
         <v>1112</v>
       </c>
     </row>
     <row r="1710" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1710" s="118"/>
+      <c r="B1710" s="122"/>
       <c r="C1710" s="11" t="s">
         <v>1113</v>
       </c>
     </row>
     <row r="1711" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1711" s="118"/>
+      <c r="B1711" s="122"/>
       <c r="C1711" s="11" t="s">
         <v>1114</v>
       </c>
     </row>
     <row r="1712" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1712" s="118"/>
+      <c r="B1712" s="122"/>
       <c r="C1712" s="11" t="s">
         <v>1115</v>
       </c>
     </row>
     <row r="1713" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1713" s="118"/>
+      <c r="B1713" s="122"/>
       <c r="C1713" s="11" t="s">
         <v>1116</v>
       </c>
     </row>
     <row r="1714" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1714" s="118"/>
+      <c r="B1714" s="122"/>
       <c r="C1714" s="11" t="s">
         <v>1117</v>
       </c>
     </row>
     <row r="1715" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1715" s="118"/>
+      <c r="B1715" s="122"/>
       <c r="C1715" s="11" t="s">
         <v>1118</v>
       </c>
     </row>
     <row r="1716" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1716" s="118"/>
+      <c r="B1716" s="122"/>
       <c r="C1716" s="11" t="s">
         <v>1119</v>
       </c>
     </row>
     <row r="1717" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1717" s="118"/>
+      <c r="B1717" s="122"/>
       <c r="C1717" s="11" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="1718" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1718" s="118"/>
+      <c r="B1718" s="122"/>
       <c r="C1718" s="11" t="s">
         <v>1121</v>
       </c>
     </row>
     <row r="1719" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1719" s="118"/>
+      <c r="B1719" s="122"/>
       <c r="C1719" s="11" t="s">
         <v>1122</v>
       </c>
     </row>
     <row r="1720" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1720" s="118"/>
+      <c r="B1720" s="122"/>
       <c r="C1720" s="35" t="s">
         <v>1123</v>
       </c>
     </row>
     <row r="1721" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B1721" s="118"/>
+      <c r="B1721" s="122"/>
       <c r="C1721" s="11"/>
     </row>
     <row r="1722" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B1722" s="118"/>
+      <c r="B1722" s="122"/>
       <c r="C1722" s="35" t="s">
         <v>2584</v>
       </c>
     </row>
     <row r="1723" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B1723" s="118"/>
+      <c r="B1723" s="122"/>
       <c r="C1723" s="35"/>
     </row>
     <row r="1724" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B1724" s="118"/>
+      <c r="B1724" s="122"/>
       <c r="C1724" s="35" t="s">
         <v>2585</v>
       </c>
     </row>
     <row r="1725" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B1725" s="118"/>
+      <c r="B1725" s="122"/>
       <c r="C1725" s="35" t="s">
         <v>2587</v>
       </c>
     </row>
     <row r="1726" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B1726" s="118"/>
+      <c r="B1726" s="122"/>
       <c r="C1726" s="35" t="s">
         <v>2590</v>
       </c>
     </row>
     <row r="1727" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B1727" s="118"/>
+      <c r="B1727" s="122"/>
       <c r="C1727" s="35" t="s">
         <v>2597</v>
       </c>
     </row>
     <row r="1728" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B1728" s="118"/>
+      <c r="B1728" s="122"/>
       <c r="C1728" s="35" t="s">
         <v>2598</v>
       </c>
@@ -36385,11 +36385,20 @@
     </row>
     <row r="1803" spans="1:3" ht="15.6">
       <c r="A1803" s="94"/>
-      <c r="B1803" s="116"/>
-      <c r="C1803" s="117"/>
+      <c r="B1803" s="120"/>
+      <c r="C1803" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A351:C351"/>
+    <mergeCell ref="A699:C699"/>
+    <mergeCell ref="A1098:C1098"/>
+    <mergeCell ref="B246:B247"/>
+    <mergeCell ref="B544:B551"/>
+    <mergeCell ref="B193:B197"/>
+    <mergeCell ref="B83:B106"/>
     <mergeCell ref="B1301:B1302"/>
     <mergeCell ref="B1549:B1554"/>
     <mergeCell ref="B1803:C1803"/>
@@ -36403,15 +36412,6 @@
     <mergeCell ref="B561:B565"/>
     <mergeCell ref="B1119:B1128"/>
     <mergeCell ref="B1698:B1728"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A351:C351"/>
-    <mergeCell ref="A699:C699"/>
-    <mergeCell ref="A1098:C1098"/>
-    <mergeCell ref="B246:B247"/>
-    <mergeCell ref="B544:B551"/>
-    <mergeCell ref="B193:B197"/>
-    <mergeCell ref="B83:B106"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C384" r:id="rId1" tooltip="https://app.pluralsight.com/course-player?clipId=fa3b6ab5-59f7-41d8-8c02-fb556f4f3a46" xr:uid="{828F1059-B150-4138-A83E-E61AA047D04C}"/>

</xml_diff>

<commit_message>
week 3 day 5
</commit_message>
<xml_diff>
--- a/TOC/ASDE 2023 - Day-wise ToC.xlsx
+++ b/TOC/ASDE 2023 - Day-wise ToC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online Training\ACE\Sapient\ASDE 2023\TOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4E5C71-97AE-44AA-A62E-17960D7ACDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D00079-A4EC-4C2D-8974-A7DF592E0D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10226,18 +10226,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -10252,6 +10240,18 @@
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -25553,10 +25553,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="120" t="s">
         <v>988</v>
       </c>
-      <c r="B1" s="116"/>
+      <c r="B1" s="121"/>
       <c r="G1" s="5"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
@@ -25579,10 +25579,10 @@
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="15.6">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="122" t="s">
         <v>990</v>
       </c>
-      <c r="B3" s="118"/>
+      <c r="B3" s="123"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -25600,7 +25600,7 @@
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:12" ht="19.2" customHeight="1">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="117" t="s">
         <v>992</v>
       </c>
       <c r="B6" s="39" t="s">
@@ -25608,19 +25608,19 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A7" s="121"/>
+      <c r="A7" s="117"/>
       <c r="B7" s="43" t="s">
         <v>994</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A8" s="121"/>
+      <c r="A8" s="117"/>
       <c r="B8" s="39" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A9" s="121"/>
+      <c r="A9" s="117"/>
       <c r="B9" s="43" t="s">
         <v>2597</v>
       </c>
@@ -25642,7 +25642,7 @@
       <c r="B12" s="39"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="121" t="s">
+      <c r="A13" s="117" t="s">
         <v>992</v>
       </c>
       <c r="B13" s="39" t="s">
@@ -25650,51 +25650,51 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="121"/>
+      <c r="A14" s="117"/>
       <c r="B14" s="43" t="s">
         <v>1711</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="121"/>
+      <c r="A15" s="117"/>
       <c r="B15" s="12" t="s">
         <v>1002</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="121"/>
+      <c r="A16" s="117"/>
       <c r="B16" s="12" t="s">
         <v>1003</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="121"/>
+      <c r="A17" s="117"/>
       <c r="B17" s="39" t="s">
         <v>2592</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="121"/>
+      <c r="A18" s="117"/>
       <c r="B18" s="12" t="s">
         <v>1006</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="121"/>
+      <c r="A19" s="117"/>
       <c r="B19" s="39" t="s">
         <v>1710</v>
       </c>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="121"/>
+      <c r="A20" s="117"/>
       <c r="B20" s="35" t="s">
         <v>2128</v>
       </c>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="121"/>
+      <c r="A21" s="117"/>
       <c r="B21" s="11" t="s">
         <v>998</v>
       </c>
@@ -25716,7 +25716,7 @@
       <c r="B24" s="39"/>
     </row>
     <row r="25" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A25" s="121" t="s">
+      <c r="A25" s="117" t="s">
         <v>992</v>
       </c>
       <c r="B25" s="39" t="s">
@@ -25724,7 +25724,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A26" s="121"/>
+      <c r="A26" s="117"/>
       <c r="B26" s="43" t="s">
         <v>2127</v>
       </c>
@@ -25760,10 +25760,10 @@
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" ht="15.6">
-      <c r="A32" s="117" t="s">
+      <c r="A32" s="122" t="s">
         <v>1007</v>
       </c>
-      <c r="B32" s="118"/>
+      <c r="B32" s="123"/>
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" ht="15.6">
@@ -25808,7 +25808,7 @@
       <c r="A39" s="3"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A40" s="121" t="s">
+      <c r="A40" s="117" t="s">
         <v>992</v>
       </c>
       <c r="B40" s="42" t="s">
@@ -25816,43 +25816,43 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A41" s="121"/>
+      <c r="A41" s="117"/>
       <c r="B41" s="12" t="s">
         <v>1015</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A42" s="121"/>
+      <c r="A42" s="117"/>
       <c r="B42" s="42" t="s">
         <v>1016</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A43" s="121"/>
+      <c r="A43" s="117"/>
       <c r="B43" s="12" t="s">
         <v>1017</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A44" s="121"/>
+      <c r="A44" s="117"/>
       <c r="B44" s="42" t="s">
         <v>1018</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A45" s="121"/>
+      <c r="A45" s="117"/>
       <c r="B45" s="12" t="s">
         <v>1019</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A46" s="121"/>
+      <c r="A46" s="117"/>
       <c r="B46" s="42" t="s">
         <v>1729</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.6" customHeight="1">
-      <c r="A47" s="121"/>
+      <c r="A47" s="117"/>
       <c r="B47" s="12" t="s">
         <v>1728</v>
       </c>
@@ -25880,7 +25880,7 @@
       <c r="B51" s="42"/>
     </row>
     <row r="52" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A52" s="121" t="s">
+      <c r="A52" s="117" t="s">
         <v>992</v>
       </c>
       <c r="B52" s="42" t="s">
@@ -25888,25 +25888,25 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A53" s="121"/>
+      <c r="A53" s="117"/>
       <c r="B53" s="12" t="s">
         <v>1009</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A54" s="121"/>
+      <c r="A54" s="117"/>
       <c r="B54" s="42" t="s">
         <v>1011</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A55" s="121"/>
+      <c r="A55" s="117"/>
       <c r="B55" s="11" t="s">
         <v>1012</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="121"/>
+      <c r="A56" s="117"/>
     </row>
     <row r="57" spans="1:2" ht="15.75" customHeight="1">
       <c r="B57" s="42" t="s">
@@ -25945,10 +25945,10 @@
       <c r="B64" s="9"/>
     </row>
     <row r="65" spans="1:2" ht="15.6">
-      <c r="A65" s="119" t="s">
+      <c r="A65" s="115" t="s">
         <v>1025</v>
       </c>
-      <c r="B65" s="120"/>
+      <c r="B65" s="116"/>
     </row>
     <row r="66" spans="1:2" ht="15.6">
       <c r="A66" s="97"/>
@@ -25971,7 +25971,7 @@
       <c r="B69" s="13"/>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="121" t="s">
+      <c r="A70" s="117" t="s">
         <v>992</v>
       </c>
       <c r="B70" s="101" t="s">
@@ -25979,7 +25979,7 @@
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="121"/>
+      <c r="A71" s="117"/>
       <c r="B71" s="11" t="s">
         <v>1028</v>
       </c>
@@ -26005,7 +26005,7 @@
       <c r="B75" s="101"/>
     </row>
     <row r="76" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A76" s="121" t="s">
+      <c r="A76" s="117" t="s">
         <v>992</v>
       </c>
       <c r="B76" s="11" t="s">
@@ -26013,7 +26013,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A77" s="121"/>
+      <c r="A77" s="117"/>
       <c r="B77" s="11" t="s">
         <v>1033</v>
       </c>
@@ -26036,7 +26036,7 @@
       <c r="B81" s="42"/>
     </row>
     <row r="82" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A82" s="121" t="s">
+      <c r="A82" s="117" t="s">
         <v>992</v>
       </c>
       <c r="B82" s="42" t="s">
@@ -26044,19 +26044,19 @@
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A83" s="121"/>
+      <c r="A83" s="117"/>
       <c r="B83" s="11" t="s">
         <v>1036</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A84" s="121"/>
+      <c r="A84" s="117"/>
       <c r="B84" s="42" t="s">
         <v>1037</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A85" s="121"/>
+      <c r="A85" s="117"/>
       <c r="B85" s="11" t="s">
         <v>1038</v>
       </c>
@@ -26092,7 +26092,7 @@
       <c r="B91" s="42"/>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" s="121" t="s">
+      <c r="A92" s="117" t="s">
         <v>992</v>
       </c>
       <c r="B92" s="42" t="s">
@@ -26100,7 +26100,7 @@
       </c>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" s="121"/>
+      <c r="A93" s="117"/>
       <c r="B93" s="35" t="s">
         <v>1038</v>
       </c>
@@ -26132,10 +26132,10 @@
       <c r="B98" s="14"/>
     </row>
     <row r="99" spans="1:2" ht="15.6">
-      <c r="A99" s="119" t="s">
+      <c r="A99" s="115" t="s">
         <v>1060</v>
       </c>
-      <c r="B99" s="120"/>
+      <c r="B99" s="116"/>
     </row>
     <row r="100" spans="1:2" ht="15.6">
       <c r="A100" s="97"/>
@@ -26154,7 +26154,7 @@
       <c r="B102" s="42"/>
     </row>
     <row r="103" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A103" s="121" t="s">
+      <c r="A103" s="117" t="s">
         <v>992</v>
       </c>
       <c r="B103" s="42" t="s">
@@ -26162,59 +26162,59 @@
       </c>
     </row>
     <row r="104" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A104" s="121"/>
+      <c r="A104" s="117"/>
       <c r="B104" s="11" t="s">
         <v>1074</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A105" s="121"/>
+      <c r="A105" s="117"/>
       <c r="B105" s="11" t="s">
         <v>1075</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A106" s="121"/>
+      <c r="A106" s="117"/>
       <c r="B106" s="11" t="s">
         <v>1076</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="1.95" customHeight="1">
-      <c r="A107" s="121"/>
+      <c r="A107" s="117"/>
       <c r="B107" s="11"/>
     </row>
     <row r="108" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A108" s="121"/>
+      <c r="A108" s="117"/>
       <c r="B108" s="11" t="s">
         <v>1077</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A109" s="121"/>
+      <c r="A109" s="117"/>
       <c r="B109" s="42" t="s">
         <v>1068</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="19.8" customHeight="1">
-      <c r="A110" s="121"/>
+      <c r="A110" s="117"/>
       <c r="B110" s="11" t="s">
         <v>1078</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A111" s="121"/>
+      <c r="A111" s="117"/>
       <c r="B111" s="42" t="s">
         <v>785</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A112" s="121"/>
+      <c r="A112" s="117"/>
       <c r="B112" s="11" t="s">
         <v>1079</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A113" s="121"/>
+      <c r="A113" s="117"/>
       <c r="B113" s="11" t="s">
         <v>1080</v>
       </c>
@@ -26235,7 +26235,7 @@
       <c r="B116" s="18"/>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="121" t="s">
+      <c r="A117" s="117" t="s">
         <v>992</v>
       </c>
       <c r="B117" s="42" t="s">
@@ -26243,25 +26243,25 @@
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A118" s="121"/>
+      <c r="A118" s="117"/>
       <c r="B118" s="11" t="s">
         <v>1087</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A119" s="121"/>
+      <c r="A119" s="117"/>
       <c r="B119" s="11" t="s">
         <v>1088</v>
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="121"/>
+      <c r="A120" s="117"/>
       <c r="B120" s="11" t="s">
         <v>1089</v>
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="121"/>
+      <c r="A121" s="117"/>
       <c r="B121" s="11" t="s">
         <v>1090</v>
       </c>
@@ -26281,7 +26281,7 @@
       <c r="B124" s="18"/>
     </row>
     <row r="125" spans="1:3" ht="18">
-      <c r="A125" s="121" t="s">
+      <c r="A125" s="117" t="s">
         <v>992</v>
       </c>
       <c r="B125" s="18" t="s">
@@ -26289,7 +26289,7 @@
       </c>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="121"/>
+      <c r="A126" s="117"/>
       <c r="B126" s="35" t="s">
         <v>2221</v>
       </c>
@@ -26324,10 +26324,10 @@
       <c r="B131" s="3"/>
     </row>
     <row r="132" spans="1:3" ht="15.6">
-      <c r="A132" s="122" t="s">
+      <c r="A132" s="118" t="s">
         <v>1092</v>
       </c>
-      <c r="B132" s="120"/>
+      <c r="B132" s="116"/>
     </row>
     <row r="133" spans="1:3" ht="15.6">
       <c r="A133" s="97"/>
@@ -26346,7 +26346,7 @@
       <c r="B135" s="104"/>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" s="121" t="s">
+      <c r="A136" s="117" t="s">
         <v>992</v>
       </c>
       <c r="B136" s="42" t="s">
@@ -26354,31 +26354,31 @@
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A137" s="121"/>
+      <c r="A137" s="117"/>
       <c r="B137" s="35" t="s">
         <v>2537</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="14.4" customHeight="1">
-      <c r="A138" s="121"/>
+      <c r="A138" s="117"/>
       <c r="B138" s="11" t="s">
         <v>1093</v>
       </c>
     </row>
     <row r="139" spans="1:3">
-      <c r="A139" s="121"/>
+      <c r="A139" s="117"/>
       <c r="B139" s="35" t="s">
         <v>2577</v>
       </c>
     </row>
     <row r="140" spans="1:3">
-      <c r="A140" s="121"/>
+      <c r="A140" s="117"/>
       <c r="B140" s="35" t="s">
         <v>2578</v>
       </c>
     </row>
     <row r="141" spans="1:3">
-      <c r="A141" s="121"/>
+      <c r="A141" s="117"/>
       <c r="B141" s="35" t="s">
         <v>2593</v>
       </c>
@@ -26422,7 +26422,7 @@
       <c r="B148" s="9"/>
     </row>
     <row r="149" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A149" s="123" t="s">
+      <c r="A149" s="119" t="s">
         <v>992</v>
       </c>
       <c r="B149" s="16" t="s">
@@ -26430,177 +26430,177 @@
       </c>
     </row>
     <row r="150" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A150" s="121"/>
+      <c r="A150" s="117"/>
       <c r="B150" s="11" t="s">
         <v>1101</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A151" s="121"/>
+      <c r="A151" s="117"/>
       <c r="B151" s="11" t="s">
         <v>1102</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A152" s="121"/>
+      <c r="A152" s="117"/>
       <c r="B152" s="11" t="s">
         <v>1103</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A153" s="121"/>
+      <c r="A153" s="117"/>
       <c r="B153" s="11" t="s">
         <v>1104</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A154" s="121"/>
+      <c r="A154" s="117"/>
       <c r="B154" s="11" t="s">
         <v>1105</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A155" s="121"/>
+      <c r="A155" s="117"/>
       <c r="B155" s="11" t="s">
         <v>1106</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A156" s="121"/>
+      <c r="A156" s="117"/>
       <c r="B156" s="11" t="s">
         <v>1107</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A157" s="121"/>
+      <c r="A157" s="117"/>
       <c r="B157" s="11" t="s">
         <v>1108</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A158" s="121"/>
+      <c r="A158" s="117"/>
       <c r="B158" s="11" t="s">
         <v>1109</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A159" s="121"/>
+      <c r="A159" s="117"/>
       <c r="B159" s="11" t="s">
         <v>1110</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A160" s="121"/>
+      <c r="A160" s="117"/>
       <c r="B160" s="11" t="s">
         <v>1111</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A161" s="121"/>
+      <c r="A161" s="117"/>
       <c r="B161" s="11" t="s">
         <v>1112</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A162" s="121"/>
+      <c r="A162" s="117"/>
       <c r="B162" s="11" t="s">
         <v>1113</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A163" s="121"/>
+      <c r="A163" s="117"/>
       <c r="B163" s="11" t="s">
         <v>1114</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A164" s="121"/>
+      <c r="A164" s="117"/>
       <c r="B164" s="11" t="s">
         <v>1115</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A165" s="121"/>
+      <c r="A165" s="117"/>
       <c r="B165" s="11" t="s">
         <v>1116</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A166" s="121"/>
+      <c r="A166" s="117"/>
       <c r="B166" s="11" t="s">
         <v>1117</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A167" s="121"/>
+      <c r="A167" s="117"/>
       <c r="B167" s="11" t="s">
         <v>1118</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A168" s="121"/>
+      <c r="A168" s="117"/>
       <c r="B168" s="11" t="s">
         <v>1119</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A169" s="121"/>
+      <c r="A169" s="117"/>
       <c r="B169" s="11" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A170" s="121"/>
+      <c r="A170" s="117"/>
       <c r="B170" s="11" t="s">
         <v>1121</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="14.4" customHeight="1">
-      <c r="A171" s="121"/>
+      <c r="A171" s="117"/>
       <c r="B171" s="11" t="s">
         <v>1122</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A172" s="121"/>
+      <c r="A172" s="117"/>
       <c r="B172" s="11"/>
     </row>
     <row r="173" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A173" s="121"/>
+      <c r="A173" s="117"/>
       <c r="B173" s="35" t="s">
         <v>2582</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A174" s="121"/>
+      <c r="A174" s="117"/>
       <c r="B174" s="35"/>
     </row>
     <row r="175" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A175" s="121"/>
+      <c r="A175" s="117"/>
       <c r="B175" s="35" t="s">
         <v>2583</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A176" s="121"/>
+      <c r="A176" s="117"/>
       <c r="B176" s="35" t="s">
         <v>2585</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A177" s="121"/>
+      <c r="A177" s="117"/>
       <c r="B177" s="35" t="s">
         <v>2588</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A178" s="121"/>
+      <c r="A178" s="117"/>
       <c r="B178" s="35" t="s">
         <v>2595</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A179" s="121"/>
+      <c r="A179" s="117"/>
       <c r="B179" s="35" t="s">
         <v>2596</v>
       </c>
@@ -26655,21 +26655,11 @@
       </c>
     </row>
     <row r="189" spans="1:2" ht="15.6">
-      <c r="A189" s="119"/>
-      <c r="B189" s="120"/>
+      <c r="A189" s="115"/>
+      <c r="B189" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A189:B189"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="A117:A121"/>
-    <mergeCell ref="A103:A113"/>
-    <mergeCell ref="A136:A141"/>
-    <mergeCell ref="A149:A179"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A32:B32"/>
@@ -26681,6 +26671,16 @@
     <mergeCell ref="A76:A77"/>
     <mergeCell ref="A52:A56"/>
     <mergeCell ref="A92:A93"/>
+    <mergeCell ref="A189:B189"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="A117:A121"/>
+    <mergeCell ref="A103:A113"/>
+    <mergeCell ref="A136:A141"/>
+    <mergeCell ref="A149:A179"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -26692,8 +26692,8 @@
   <dimension ref="A1:M1792"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A756" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D792" sqref="D792"/>
+      <pane ySplit="2" topLeftCell="A1567" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D899" sqref="D899"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -26706,11 +26706,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="120" t="s">
         <v>988</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
       <c r="H1" s="5"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
@@ -26736,11 +26736,11 @@
       <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" ht="12" customHeight="1">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="122" t="s">
         <v>990</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -27214,7 +27214,7 @@
       <c r="C82" s="12"/>
     </row>
     <row r="83" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B83" s="121" t="s">
+      <c r="B83" s="117" t="s">
         <v>992</v>
       </c>
       <c r="C83" s="39" t="s">
@@ -27222,143 +27222,143 @@
       </c>
     </row>
     <row r="84" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B84" s="121"/>
+      <c r="B84" s="117"/>
       <c r="C84" s="12" t="s">
         <v>994</v>
       </c>
     </row>
     <row r="85" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B85" s="121"/>
+      <c r="B85" s="117"/>
       <c r="C85" s="39" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="86" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B86" s="121"/>
+      <c r="B86" s="117"/>
       <c r="C86" s="43" t="s">
         <v>2670</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B87" s="121"/>
+      <c r="B87" s="117"/>
       <c r="C87" s="39" t="s">
         <v>2651</v>
       </c>
     </row>
     <row r="88" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B88" s="121"/>
+      <c r="B88" s="117"/>
       <c r="C88" s="12" t="s">
         <v>2661</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B89" s="121"/>
+      <c r="B89" s="117"/>
       <c r="C89" s="43" t="s">
         <v>2662</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B90" s="121"/>
+      <c r="B90" s="117"/>
       <c r="C90" s="12" t="s">
         <v>2663</v>
       </c>
     </row>
     <row r="91" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B91" s="121"/>
+      <c r="B91" s="117"/>
       <c r="C91" s="113" t="s">
         <v>2652</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B92" s="121"/>
+      <c r="B92" s="117"/>
       <c r="C92" s="113" t="s">
         <v>2653</v>
       </c>
     </row>
     <row r="93" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B93" s="121"/>
+      <c r="B93" s="117"/>
       <c r="C93" s="113" t="s">
         <v>2654</v>
       </c>
     </row>
     <row r="94" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B94" s="121"/>
+      <c r="B94" s="117"/>
       <c r="C94" s="39" t="s">
         <v>2656</v>
       </c>
     </row>
     <row r="95" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B95" s="121"/>
+      <c r="B95" s="117"/>
       <c r="C95" s="113" t="s">
         <v>2655</v>
       </c>
     </row>
     <row r="96" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B96" s="121"/>
+      <c r="B96" s="117"/>
       <c r="C96" t="s">
         <v>2657</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B97" s="121"/>
+      <c r="B97" s="117"/>
       <c r="C97" s="39" t="s">
         <v>2671</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B98" s="121"/>
+      <c r="B98" s="117"/>
       <c r="C98" s="43" t="s">
         <v>2658</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B99" s="121"/>
+      <c r="B99" s="117"/>
       <c r="C99" s="43" t="s">
         <v>2659</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B100" s="121"/>
+      <c r="B100" s="117"/>
       <c r="C100" s="43" t="s">
         <v>2660</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B101" s="121"/>
+      <c r="B101" s="117"/>
       <c r="C101" s="39" t="s">
         <v>2666</v>
       </c>
     </row>
     <row r="102" spans="1:9">
-      <c r="B102" s="121"/>
+      <c r="B102" s="117"/>
       <c r="C102" s="43" t="s">
         <v>2664</v>
       </c>
       <c r="I102" s="2"/>
     </row>
     <row r="103" spans="1:9">
-      <c r="B103" s="121"/>
+      <c r="B103" s="117"/>
       <c r="C103" s="43" t="s">
         <v>2665</v>
       </c>
       <c r="I103" s="2"/>
     </row>
     <row r="104" spans="1:9">
-      <c r="B104" s="121"/>
+      <c r="B104" s="117"/>
       <c r="C104" s="39" t="s">
         <v>2668</v>
       </c>
       <c r="I104" s="2"/>
     </row>
     <row r="105" spans="1:9">
-      <c r="B105" s="121"/>
+      <c r="B105" s="117"/>
       <c r="C105" s="114" t="s">
         <v>2667</v>
       </c>
       <c r="I105" s="2"/>
     </row>
     <row r="106" spans="1:9">
-      <c r="B106" s="121"/>
+      <c r="B106" s="117"/>
       <c r="C106" s="114" t="s">
         <v>2669</v>
       </c>
@@ -27725,7 +27725,7 @@
       <c r="I168" s="2"/>
     </row>
     <row r="169" spans="2:9">
-      <c r="B169" s="121" t="s">
+      <c r="B169" s="117" t="s">
         <v>992</v>
       </c>
       <c r="C169" s="39" t="s">
@@ -27734,21 +27734,21 @@
       <c r="I169" s="2"/>
     </row>
     <row r="170" spans="2:9">
-      <c r="B170" s="121"/>
+      <c r="B170" s="117"/>
       <c r="C170" s="43" t="s">
         <v>1711</v>
       </c>
       <c r="I170" s="2"/>
     </row>
     <row r="171" spans="2:9">
-      <c r="B171" s="121"/>
+      <c r="B171" s="117"/>
       <c r="C171" s="12" t="s">
         <v>1002</v>
       </c>
       <c r="I171" s="2"/>
     </row>
     <row r="172" spans="2:9">
-      <c r="B172" s="121"/>
+      <c r="B172" s="117"/>
       <c r="C172" s="12" t="s">
         <v>1003</v>
       </c>
@@ -27868,7 +27868,7 @@
       <c r="I192" s="2"/>
     </row>
     <row r="193" spans="1:9" ht="14.4" customHeight="1">
-      <c r="B193" s="121" t="s">
+      <c r="B193" s="117" t="s">
         <v>992</v>
       </c>
       <c r="C193" s="39" t="s">
@@ -27877,28 +27877,28 @@
       <c r="I193" s="2"/>
     </row>
     <row r="194" spans="1:9" ht="14.4" customHeight="1">
-      <c r="B194" s="121"/>
+      <c r="B194" s="117"/>
       <c r="C194" s="12" t="s">
         <v>1006</v>
       </c>
       <c r="I194" s="2"/>
     </row>
     <row r="195" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B195" s="121"/>
+      <c r="B195" s="117"/>
       <c r="C195" s="39" t="s">
         <v>1710</v>
       </c>
       <c r="I195" s="2"/>
     </row>
     <row r="196" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B196" s="121"/>
+      <c r="B196" s="117"/>
       <c r="C196" s="35" t="s">
         <v>2128</v>
       </c>
       <c r="I196" s="2"/>
     </row>
     <row r="197" spans="1:9" ht="15.6" customHeight="1">
-      <c r="B197" s="121"/>
+      <c r="B197" s="117"/>
       <c r="C197" s="11" t="s">
         <v>998</v>
       </c>
@@ -28252,7 +28252,7 @@
       <c r="I245" s="2"/>
     </row>
     <row r="246" spans="1:9">
-      <c r="B246" s="121" t="s">
+      <c r="B246" s="117" t="s">
         <v>992</v>
       </c>
       <c r="C246" s="39" t="s">
@@ -28261,7 +28261,7 @@
       <c r="I246" s="2"/>
     </row>
     <row r="247" spans="1:9">
-      <c r="B247" s="121"/>
+      <c r="B247" s="117"/>
       <c r="C247" s="43" t="s">
         <v>2127</v>
       </c>
@@ -28773,11 +28773,11 @@
       <c r="I350" s="2"/>
     </row>
     <row r="351" spans="1:9" ht="15.6">
-      <c r="A351" s="117" t="s">
+      <c r="A351" s="122" t="s">
         <v>1007</v>
       </c>
-      <c r="B351" s="117"/>
-      <c r="C351" s="117"/>
+      <c r="B351" s="122"/>
+      <c r="C351" s="122"/>
       <c r="I351" s="2"/>
     </row>
     <row r="352" spans="1:9" ht="15">
@@ -29805,7 +29805,7 @@
       <c r="C543" s="12"/>
     </row>
     <row r="544" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B544" s="121" t="s">
+      <c r="B544" s="117" t="s">
         <v>992</v>
       </c>
       <c r="C544" s="42" t="s">
@@ -29813,43 +29813,43 @@
       </c>
     </row>
     <row r="545" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B545" s="121"/>
+      <c r="B545" s="117"/>
       <c r="C545" s="12" t="s">
         <v>1015</v>
       </c>
     </row>
     <row r="546" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B546" s="121"/>
+      <c r="B546" s="117"/>
       <c r="C546" s="42" t="s">
         <v>1016</v>
       </c>
     </row>
     <row r="547" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B547" s="121"/>
+      <c r="B547" s="117"/>
       <c r="C547" s="12" t="s">
         <v>1017</v>
       </c>
     </row>
     <row r="548" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B548" s="121"/>
+      <c r="B548" s="117"/>
       <c r="C548" s="42" t="s">
         <v>1018</v>
       </c>
     </row>
     <row r="549" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B549" s="121"/>
+      <c r="B549" s="117"/>
       <c r="C549" s="12" t="s">
         <v>1019</v>
       </c>
     </row>
     <row r="550" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B550" s="121"/>
+      <c r="B550" s="117"/>
       <c r="C550" s="42" t="s">
         <v>1729</v>
       </c>
     </row>
     <row r="551" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B551" s="121"/>
+      <c r="B551" s="117"/>
       <c r="C551" s="12" t="s">
         <v>1728</v>
       </c>
@@ -29904,7 +29904,7 @@
       <c r="C560" s="12"/>
     </row>
     <row r="561" spans="1:9" ht="14.4" customHeight="1">
-      <c r="B561" s="121" t="s">
+      <c r="B561" s="117" t="s">
         <v>992</v>
       </c>
       <c r="C561" s="42" t="s">
@@ -29912,25 +29912,25 @@
       </c>
     </row>
     <row r="562" spans="1:9" ht="14.4" customHeight="1">
-      <c r="B562" s="121"/>
+      <c r="B562" s="117"/>
       <c r="C562" s="12" t="s">
         <v>1009</v>
       </c>
     </row>
     <row r="563" spans="1:9">
-      <c r="B563" s="121"/>
+      <c r="B563" s="117"/>
       <c r="C563" s="42" t="s">
         <v>1011</v>
       </c>
     </row>
     <row r="564" spans="1:9" ht="14.4" customHeight="1">
-      <c r="B564" s="121"/>
+      <c r="B564" s="117"/>
       <c r="C564" s="11" t="s">
         <v>1012</v>
       </c>
     </row>
     <row r="565" spans="1:9" ht="14.4" customHeight="1">
-      <c r="B565" s="121"/>
+      <c r="B565" s="117"/>
     </row>
     <row r="566" spans="1:9" ht="15.6">
       <c r="B566" s="10"/>
@@ -30680,11 +30680,11 @@
       <c r="C698" s="11"/>
     </row>
     <row r="699" spans="1:3" ht="13.8" customHeight="1">
-      <c r="A699" s="117" t="s">
+      <c r="A699" s="122" t="s">
         <v>1025</v>
       </c>
-      <c r="B699" s="117"/>
-      <c r="C699" s="117"/>
+      <c r="B699" s="122"/>
+      <c r="C699" s="122"/>
     </row>
     <row r="700" spans="1:3" ht="15.6">
       <c r="A700" s="99"/>
@@ -31202,7 +31202,7 @@
       <c r="C799" s="35"/>
     </row>
     <row r="800" spans="1:4">
-      <c r="B800" s="121" t="s">
+      <c r="B800" s="117" t="s">
         <v>992</v>
       </c>
       <c r="C800" s="42" t="s">
@@ -31210,7 +31210,7 @@
       </c>
     </row>
     <row r="801" spans="1:3">
-      <c r="B801" s="121"/>
+      <c r="B801" s="117"/>
       <c r="C801" s="35" t="s">
         <v>1036</v>
       </c>
@@ -32614,11 +32614,11 @@
       <c r="C1086" s="35"/>
     </row>
     <row r="1087" spans="1:3" ht="15.6">
-      <c r="A1087" s="117" t="s">
+      <c r="A1087" s="122" t="s">
         <v>1060</v>
       </c>
-      <c r="B1087" s="117"/>
-      <c r="C1087" s="117"/>
+      <c r="B1087" s="122"/>
+      <c r="C1087" s="122"/>
     </row>
     <row r="1088" spans="1:3">
       <c r="C1088" s="35"/>
@@ -32717,7 +32717,7 @@
       <c r="C1107" s="35"/>
     </row>
     <row r="1108" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1108" s="121" t="s">
+      <c r="B1108" s="117" t="s">
         <v>992</v>
       </c>
       <c r="C1108" s="42" t="s">
@@ -32725,56 +32725,56 @@
       </c>
     </row>
     <row r="1109" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1109" s="121"/>
+      <c r="B1109" s="117"/>
       <c r="C1109" s="35" t="s">
         <v>1074</v>
       </c>
     </row>
     <row r="1110" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1110" s="121"/>
+      <c r="B1110" s="117"/>
       <c r="C1110" s="35" t="s">
         <v>1075</v>
       </c>
     </row>
     <row r="1111" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1111" s="121"/>
+      <c r="B1111" s="117"/>
       <c r="C1111" s="35" t="s">
         <v>1076</v>
       </c>
     </row>
     <row r="1112" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1112" s="121"/>
+      <c r="B1112" s="117"/>
       <c r="C1112" s="35" t="s">
         <v>1077</v>
       </c>
     </row>
     <row r="1113" spans="1:4" ht="15.6" customHeight="1">
-      <c r="B1113" s="121"/>
+      <c r="B1113" s="117"/>
       <c r="C1113" s="42" t="s">
         <v>1068</v>
       </c>
     </row>
     <row r="1114" spans="1:4" ht="16.8" customHeight="1">
-      <c r="B1114" s="121"/>
+      <c r="B1114" s="117"/>
       <c r="C1114" s="35" t="s">
         <v>1078</v>
       </c>
     </row>
     <row r="1115" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1115" s="121"/>
+      <c r="B1115" s="117"/>
       <c r="C1115" s="42" t="s">
         <v>785</v>
       </c>
     </row>
     <row r="1116" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1116" s="121"/>
+      <c r="B1116" s="117"/>
       <c r="C1116" s="35" t="s">
         <v>1079</v>
       </c>
       <c r="D1116" s="108"/>
     </row>
     <row r="1117" spans="1:4" ht="14.4" customHeight="1">
-      <c r="B1117" s="121"/>
+      <c r="B1117" s="117"/>
       <c r="C1117" s="35" t="s">
         <v>1080</v>
       </c>
@@ -33142,7 +33142,7 @@
       <c r="C1190" s="35"/>
     </row>
     <row r="1191" spans="1:3" ht="18">
-      <c r="B1191" s="121" t="s">
+      <c r="B1191" s="117" t="s">
         <v>992</v>
       </c>
       <c r="C1191" s="18" t="s">
@@ -33150,25 +33150,25 @@
       </c>
     </row>
     <row r="1192" spans="1:3">
-      <c r="B1192" s="121"/>
+      <c r="B1192" s="117"/>
       <c r="C1192" s="35" t="s">
         <v>1087</v>
       </c>
     </row>
     <row r="1193" spans="1:3">
-      <c r="B1193" s="121"/>
+      <c r="B1193" s="117"/>
       <c r="C1193" s="35" t="s">
         <v>1088</v>
       </c>
     </row>
     <row r="1194" spans="1:3">
-      <c r="B1194" s="121"/>
+      <c r="B1194" s="117"/>
       <c r="C1194" s="35" t="s">
         <v>1089</v>
       </c>
     </row>
     <row r="1195" spans="1:3">
-      <c r="B1195" s="121"/>
+      <c r="B1195" s="117"/>
       <c r="C1195" s="35" t="s">
         <v>1090</v>
       </c>
@@ -33705,7 +33705,7 @@
       <c r="C1289" s="42"/>
     </row>
     <row r="1290" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1290" s="121" t="s">
+      <c r="B1290" s="117" t="s">
         <v>992</v>
       </c>
       <c r="C1290" s="42" t="s">
@@ -33713,7 +33713,7 @@
       </c>
     </row>
     <row r="1291" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1291" s="121"/>
+      <c r="B1291" s="117"/>
       <c r="C1291" s="35" t="s">
         <v>2536</v>
       </c>
@@ -34588,11 +34588,11 @@
       <c r="C1479" s="35"/>
     </row>
     <row r="1480" spans="1:4" ht="15.6">
-      <c r="A1480" s="117" t="s">
+      <c r="A1480" s="122" t="s">
         <v>1092</v>
       </c>
-      <c r="B1480" s="117"/>
-      <c r="C1480" s="117"/>
+      <c r="B1480" s="122"/>
+      <c r="C1480" s="122"/>
     </row>
     <row r="1481" spans="1:4" ht="15.6">
       <c r="A1481" s="99"/>
@@ -34925,7 +34925,7 @@
       <c r="C1537" s="35"/>
     </row>
     <row r="1538" spans="1:3" ht="14.4" customHeight="1">
-      <c r="B1538" s="121" t="s">
+      <c r="B1538" s="117" t="s">
         <v>992</v>
       </c>
       <c r="C1538" s="42" t="s">
@@ -34933,31 +34933,31 @@
       </c>
     </row>
     <row r="1539" spans="1:3" ht="14.4" customHeight="1">
-      <c r="B1539" s="121"/>
+      <c r="B1539" s="117"/>
       <c r="C1539" s="35" t="s">
         <v>2537</v>
       </c>
     </row>
     <row r="1540" spans="1:3" ht="14.4" customHeight="1">
-      <c r="B1540" s="121"/>
+      <c r="B1540" s="117"/>
       <c r="C1540" s="11" t="s">
         <v>1093</v>
       </c>
     </row>
     <row r="1541" spans="1:3" ht="15.6" customHeight="1">
-      <c r="B1541" s="121"/>
+      <c r="B1541" s="117"/>
       <c r="C1541" s="35" t="s">
         <v>2577</v>
       </c>
     </row>
     <row r="1542" spans="1:3" ht="15.6" customHeight="1">
-      <c r="B1542" s="121"/>
+      <c r="B1542" s="117"/>
       <c r="C1542" s="35" t="s">
         <v>2578</v>
       </c>
     </row>
     <row r="1543" spans="1:3" ht="15.6" customHeight="1">
-      <c r="B1543" s="121"/>
+      <c r="B1543" s="117"/>
       <c r="C1543" s="35" t="s">
         <v>2593</v>
       </c>
@@ -35711,7 +35711,7 @@
       <c r="C1686" s="11"/>
     </row>
     <row r="1687" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1687" s="121" t="s">
+      <c r="B1687" s="117" t="s">
         <v>992</v>
       </c>
       <c r="C1687" s="46" t="s">
@@ -35719,177 +35719,177 @@
       </c>
     </row>
     <row r="1688" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1688" s="121"/>
+      <c r="B1688" s="117"/>
       <c r="C1688" s="11" t="s">
         <v>1101</v>
       </c>
     </row>
     <row r="1689" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1689" s="121"/>
+      <c r="B1689" s="117"/>
       <c r="C1689" s="11" t="s">
         <v>1102</v>
       </c>
     </row>
     <row r="1690" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1690" s="121"/>
+      <c r="B1690" s="117"/>
       <c r="C1690" s="11" t="s">
         <v>1103</v>
       </c>
     </row>
     <row r="1691" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1691" s="121"/>
+      <c r="B1691" s="117"/>
       <c r="C1691" s="11" t="s">
         <v>1104</v>
       </c>
     </row>
     <row r="1692" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1692" s="121"/>
+      <c r="B1692" s="117"/>
       <c r="C1692" s="11" t="s">
         <v>1105</v>
       </c>
     </row>
     <row r="1693" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1693" s="121"/>
+      <c r="B1693" s="117"/>
       <c r="C1693" s="11" t="s">
         <v>1106</v>
       </c>
     </row>
     <row r="1694" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1694" s="121"/>
+      <c r="B1694" s="117"/>
       <c r="C1694" s="11" t="s">
         <v>1107</v>
       </c>
     </row>
     <row r="1695" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1695" s="121"/>
+      <c r="B1695" s="117"/>
       <c r="C1695" s="11" t="s">
         <v>1108</v>
       </c>
     </row>
     <row r="1696" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1696" s="121"/>
+      <c r="B1696" s="117"/>
       <c r="C1696" s="11" t="s">
         <v>1109</v>
       </c>
     </row>
     <row r="1697" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1697" s="121"/>
+      <c r="B1697" s="117"/>
       <c r="C1697" s="11" t="s">
         <v>1110</v>
       </c>
     </row>
     <row r="1698" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1698" s="121"/>
+      <c r="B1698" s="117"/>
       <c r="C1698" s="11" t="s">
         <v>1111</v>
       </c>
     </row>
     <row r="1699" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1699" s="121"/>
+      <c r="B1699" s="117"/>
       <c r="C1699" s="11" t="s">
         <v>1112</v>
       </c>
     </row>
     <row r="1700" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1700" s="121"/>
+      <c r="B1700" s="117"/>
       <c r="C1700" s="11" t="s">
         <v>1113</v>
       </c>
     </row>
     <row r="1701" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1701" s="121"/>
+      <c r="B1701" s="117"/>
       <c r="C1701" s="11" t="s">
         <v>1114</v>
       </c>
     </row>
     <row r="1702" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1702" s="121"/>
+      <c r="B1702" s="117"/>
       <c r="C1702" s="11" t="s">
         <v>1115</v>
       </c>
     </row>
     <row r="1703" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1703" s="121"/>
+      <c r="B1703" s="117"/>
       <c r="C1703" s="11" t="s">
         <v>1116</v>
       </c>
     </row>
     <row r="1704" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1704" s="121"/>
+      <c r="B1704" s="117"/>
       <c r="C1704" s="11" t="s">
         <v>1117</v>
       </c>
     </row>
     <row r="1705" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1705" s="121"/>
+      <c r="B1705" s="117"/>
       <c r="C1705" s="11" t="s">
         <v>1118</v>
       </c>
     </row>
     <row r="1706" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1706" s="121"/>
+      <c r="B1706" s="117"/>
       <c r="C1706" s="11" t="s">
         <v>1119</v>
       </c>
     </row>
     <row r="1707" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1707" s="121"/>
+      <c r="B1707" s="117"/>
       <c r="C1707" s="11" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="1708" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1708" s="121"/>
+      <c r="B1708" s="117"/>
       <c r="C1708" s="11" t="s">
         <v>1121</v>
       </c>
     </row>
     <row r="1709" spans="2:3" ht="14.4" customHeight="1">
-      <c r="B1709" s="121"/>
+      <c r="B1709" s="117"/>
       <c r="C1709" s="35" t="s">
         <v>1122</v>
       </c>
     </row>
     <row r="1710" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B1710" s="121"/>
+      <c r="B1710" s="117"/>
       <c r="C1710" s="11"/>
     </row>
     <row r="1711" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B1711" s="121"/>
+      <c r="B1711" s="117"/>
       <c r="C1711" s="35" t="s">
         <v>2582</v>
       </c>
     </row>
     <row r="1712" spans="2:3" ht="15.6" customHeight="1">
-      <c r="B1712" s="121"/>
+      <c r="B1712" s="117"/>
       <c r="C1712" s="35"/>
     </row>
     <row r="1713" spans="1:3" ht="15.6" customHeight="1">
-      <c r="B1713" s="121"/>
+      <c r="B1713" s="117"/>
       <c r="C1713" s="35" t="s">
         <v>2583</v>
       </c>
     </row>
     <row r="1714" spans="1:3" ht="15.6" customHeight="1">
-      <c r="B1714" s="121"/>
+      <c r="B1714" s="117"/>
       <c r="C1714" s="35" t="s">
         <v>2585</v>
       </c>
     </row>
     <row r="1715" spans="1:3" ht="15.6" customHeight="1">
-      <c r="B1715" s="121"/>
+      <c r="B1715" s="117"/>
       <c r="C1715" s="35" t="s">
         <v>2588</v>
       </c>
     </row>
     <row r="1716" spans="1:3" ht="15.6" customHeight="1">
-      <c r="B1716" s="121"/>
+      <c r="B1716" s="117"/>
       <c r="C1716" s="35" t="s">
         <v>2595</v>
       </c>
     </row>
     <row r="1717" spans="1:3" ht="15.6" customHeight="1">
-      <c r="B1717" s="121"/>
+      <c r="B1717" s="117"/>
       <c r="C1717" s="35" t="s">
         <v>2596</v>
       </c>
@@ -36314,20 +36314,11 @@
     </row>
     <row r="1792" spans="1:3" ht="15.6">
       <c r="A1792" s="94"/>
-      <c r="B1792" s="119"/>
-      <c r="C1792" s="120"/>
+      <c r="B1792" s="115"/>
+      <c r="C1792" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A351:C351"/>
-    <mergeCell ref="A699:C699"/>
-    <mergeCell ref="A1087:C1087"/>
-    <mergeCell ref="B246:B247"/>
-    <mergeCell ref="B544:B551"/>
-    <mergeCell ref="B193:B197"/>
-    <mergeCell ref="B83:B106"/>
     <mergeCell ref="B1290:B1291"/>
     <mergeCell ref="B1538:B1543"/>
     <mergeCell ref="B1792:C1792"/>
@@ -36338,6 +36329,15 @@
     <mergeCell ref="B561:B565"/>
     <mergeCell ref="B1108:B1117"/>
     <mergeCell ref="B1687:B1717"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A351:C351"/>
+    <mergeCell ref="A699:C699"/>
+    <mergeCell ref="A1087:C1087"/>
+    <mergeCell ref="B246:B247"/>
+    <mergeCell ref="B544:B551"/>
+    <mergeCell ref="B193:B197"/>
+    <mergeCell ref="B83:B106"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C384" r:id="rId1" tooltip="https://app.pluralsight.com/course-player?clipId=fa3b6ab5-59f7-41d8-8c02-fb556f4f3a46" xr:uid="{828F1059-B150-4138-A83E-E61AA047D04C}"/>

</xml_diff>